<commit_message>
gets students, get one student
</commit_message>
<xml_diff>
--- a/groupe_projet/projets.xlsx
+++ b/groupe_projet/projets.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\workspace\2.Trainning\iscae\JS\iscae_m1\groupe_projet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33F07FDC-5613-4D8C-88CD-034EABA1E747}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A30CDCD-6D5F-4BC2-B8C1-90A4DD27B57B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{A06B96B0-DA0B-46D0-B1EE-E2CD1AE260FB}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="49">
   <si>
     <t>Groupe</t>
   </si>
@@ -158,9 +158,6 @@
   </si>
   <si>
     <t>Gestion employés</t>
-  </si>
-  <si>
-    <t>Gestion parc auto</t>
   </si>
   <si>
     <t xml:space="preserve">Pas de Spring BOOT ni ANGULAR OU framework </t>
@@ -206,6 +203,12 @@
   </si>
   <si>
     <t>Gestion Hotels</t>
+  </si>
+  <si>
+    <t>IE 18674</t>
+  </si>
+  <si>
+    <t>Gestion bibliothèque</t>
   </si>
 </sst>
 </file>
@@ -278,8 +281,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{88568CE5-77DD-4A7C-8FE0-47C36F793209}" name="Table1" displayName="Table1" ref="A2:D35" totalsRowShown="0">
-  <autoFilter ref="A2:D35" xr:uid="{88568CE5-77DD-4A7C-8FE0-47C36F793209}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{88568CE5-77DD-4A7C-8FE0-47C36F793209}" name="Table1" displayName="Table1" ref="A2:D36" totalsRowShown="0">
+  <autoFilter ref="A2:D36" xr:uid="{88568CE5-77DD-4A7C-8FE0-47C36F793209}"/>
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{70F8D69D-AC1A-4FD0-A604-DF009531651D}" name="Groupe"/>
     <tableColumn id="2" xr3:uid="{A0589071-5C77-4331-A6FE-3323A6589426}" name="Etudiant "/>
@@ -587,10 +590,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{27FC3ED8-FCCE-4891-A526-28F3009172D0}">
-  <dimension ref="A2:D35"/>
+  <dimension ref="A2:D36"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -623,7 +626,7 @@
         <v>4</v>
       </c>
       <c r="D3" t="s">
-        <v>41</v>
+        <v>48</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
@@ -634,7 +637,7 @@
         <v>5</v>
       </c>
       <c r="D4" t="s">
-        <v>41</v>
+        <v>48</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
@@ -645,7 +648,7 @@
         <v>6</v>
       </c>
       <c r="D5" t="s">
-        <v>41</v>
+        <v>48</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
@@ -656,7 +659,7 @@
         <v>7</v>
       </c>
       <c r="D6" t="s">
-        <v>41</v>
+        <v>48</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
@@ -667,7 +670,7 @@
         <v>8</v>
       </c>
       <c r="D7" t="s">
-        <v>41</v>
+        <v>48</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
@@ -741,7 +744,7 @@
         <v>3</v>
       </c>
       <c r="C14" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D14" t="s">
         <v>40</v>
@@ -749,13 +752,13 @@
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C15" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D15" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.3">
@@ -763,7 +766,7 @@
         <v>4</v>
       </c>
       <c r="C16" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D16" t="s">
         <v>39</v>
@@ -774,7 +777,7 @@
         <v>4</v>
       </c>
       <c r="C17" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D17" t="s">
         <v>39</v>
@@ -785,7 +788,7 @@
         <v>4</v>
       </c>
       <c r="C18" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="D18" t="s">
         <v>39</v>
@@ -796,7 +799,7 @@
         <v>4</v>
       </c>
       <c r="C19" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="D19" t="s">
         <v>39</v>
@@ -804,13 +807,13 @@
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C20" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="D20" t="s">
-        <v>39</v>
+        <v>44</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.3">
@@ -818,18 +821,18 @@
         <v>5</v>
       </c>
       <c r="C21" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D21" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A22">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C22" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D22" t="s">
         <v>45</v>
@@ -840,10 +843,10 @@
         <v>6</v>
       </c>
       <c r="C23" t="s">
-        <v>25</v>
+        <v>14</v>
       </c>
       <c r="D23" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.3">
@@ -854,7 +857,7 @@
         <v>26</v>
       </c>
       <c r="D24" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.3">
@@ -865,7 +868,7 @@
         <v>27</v>
       </c>
       <c r="D25" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.3">
@@ -876,7 +879,7 @@
         <v>28</v>
       </c>
       <c r="D26" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.3">
@@ -887,7 +890,7 @@
         <v>29</v>
       </c>
       <c r="D27" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.3">
@@ -898,7 +901,7 @@
         <v>30</v>
       </c>
       <c r="D28" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.3">
@@ -909,7 +912,7 @@
         <v>31</v>
       </c>
       <c r="D29" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.3">
@@ -917,21 +920,21 @@
         <v>7</v>
       </c>
       <c r="C30" t="s">
-        <v>32</v>
+        <v>47</v>
       </c>
       <c r="D30" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A31">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C31" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D31" t="s">
-        <v>37</v>
+        <v>46</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.3">
@@ -939,7 +942,7 @@
         <v>8</v>
       </c>
       <c r="C32" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D32" t="s">
         <v>37</v>
@@ -950,7 +953,7 @@
         <v>8</v>
       </c>
       <c r="C33" t="s">
-        <v>19</v>
+        <v>34</v>
       </c>
       <c r="D33" t="s">
         <v>37</v>
@@ -961,7 +964,7 @@
         <v>8</v>
       </c>
       <c r="C34" t="s">
-        <v>35</v>
+        <v>19</v>
       </c>
       <c r="D34" t="s">
         <v>37</v>
@@ -972,9 +975,20 @@
         <v>8</v>
       </c>
       <c r="C35" t="s">
+        <v>35</v>
+      </c>
+      <c r="D35" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A36">
+        <v>8</v>
+      </c>
+      <c r="C36" t="s">
         <v>36</v>
       </c>
-      <c r="D35" t="s">
+      <c r="D36" t="s">
         <v>37</v>
       </c>
     </row>
@@ -1003,17 +1017,17 @@
   <sheetData>
     <row r="2" spans="1:1" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
terminer les actions rest pour etudiant
</commit_message>
<xml_diff>
--- a/groupe_projet/projets.xlsx
+++ b/groupe_projet/projets.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\workspace\2.Trainning\iscae\JS\iscae_m1\groupe_projet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A30CDCD-6D5F-4BC2-B8C1-90A4DD27B57B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8934A8E4-8C1A-425E-89E9-0D6366FD84BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{A06B96B0-DA0B-46D0-B1EE-E2CD1AE260FB}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="53">
   <si>
     <t>Groupe</t>
   </si>
@@ -209,6 +209,18 @@
   </si>
   <si>
     <t>Gestion bibliothèque</t>
+  </si>
+  <si>
+    <t>IP 18732</t>
+  </si>
+  <si>
+    <t>IP 18114</t>
+  </si>
+  <si>
+    <t>IP 18111</t>
+  </si>
+  <si>
+    <t>Gestion de transfert d'argent</t>
   </si>
 </sst>
 </file>
@@ -281,8 +293,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{88568CE5-77DD-4A7C-8FE0-47C36F793209}" name="Table1" displayName="Table1" ref="A2:D36" totalsRowShown="0">
-  <autoFilter ref="A2:D36" xr:uid="{88568CE5-77DD-4A7C-8FE0-47C36F793209}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{88568CE5-77DD-4A7C-8FE0-47C36F793209}" name="Table1" displayName="Table1" ref="A2:D39" totalsRowShown="0">
+  <autoFilter ref="A2:D39" xr:uid="{88568CE5-77DD-4A7C-8FE0-47C36F793209}"/>
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{70F8D69D-AC1A-4FD0-A604-DF009531651D}" name="Groupe"/>
     <tableColumn id="2" xr3:uid="{A0589071-5C77-4331-A6FE-3323A6589426}" name="Etudiant "/>
@@ -590,10 +602,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{27FC3ED8-FCCE-4891-A526-28F3009172D0}">
-  <dimension ref="A2:D36"/>
+  <dimension ref="A2:D39"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+    <sheetView tabSelected="1" topLeftCell="A28" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="D39" sqref="D39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -744,7 +756,7 @@
         <v>3</v>
       </c>
       <c r="C14" t="s">
-        <v>15</v>
+        <v>49</v>
       </c>
       <c r="D14" t="s">
         <v>40</v>
@@ -752,13 +764,13 @@
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C15" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D15" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.3">
@@ -766,7 +778,7 @@
         <v>4</v>
       </c>
       <c r="C16" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D16" t="s">
         <v>39</v>
@@ -777,7 +789,7 @@
         <v>4</v>
       </c>
       <c r="C17" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D17" t="s">
         <v>39</v>
@@ -788,7 +800,7 @@
         <v>4</v>
       </c>
       <c r="C18" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="D18" t="s">
         <v>39</v>
@@ -799,7 +811,7 @@
         <v>4</v>
       </c>
       <c r="C19" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="D19" t="s">
         <v>39</v>
@@ -807,13 +819,13 @@
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C20" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="D20" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.3">
@@ -821,7 +833,7 @@
         <v>5</v>
       </c>
       <c r="C21" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D21" t="s">
         <v>44</v>
@@ -829,13 +841,13 @@
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A22">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C22" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D22" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.3">
@@ -843,7 +855,7 @@
         <v>6</v>
       </c>
       <c r="C23" t="s">
-        <v>14</v>
+        <v>25</v>
       </c>
       <c r="D23" t="s">
         <v>45</v>
@@ -854,7 +866,7 @@
         <v>6</v>
       </c>
       <c r="C24" t="s">
-        <v>26</v>
+        <v>14</v>
       </c>
       <c r="D24" t="s">
         <v>45</v>
@@ -864,8 +876,8 @@
       <c r="A25">
         <v>6</v>
       </c>
-      <c r="B25" t="s">
-        <v>27</v>
+      <c r="C25" t="s">
+        <v>26</v>
       </c>
       <c r="D25" t="s">
         <v>45</v>
@@ -875,8 +887,8 @@
       <c r="A26">
         <v>6</v>
       </c>
-      <c r="C26" t="s">
-        <v>28</v>
+      <c r="B26" t="s">
+        <v>27</v>
       </c>
       <c r="D26" t="s">
         <v>45</v>
@@ -884,13 +896,13 @@
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A27">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C27" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D27" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.3">
@@ -898,7 +910,7 @@
         <v>7</v>
       </c>
       <c r="C28" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D28" t="s">
         <v>46</v>
@@ -909,7 +921,7 @@
         <v>7</v>
       </c>
       <c r="C29" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D29" t="s">
         <v>46</v>
@@ -920,7 +932,7 @@
         <v>7</v>
       </c>
       <c r="C30" t="s">
-        <v>47</v>
+        <v>31</v>
       </c>
       <c r="D30" t="s">
         <v>46</v>
@@ -931,7 +943,7 @@
         <v>7</v>
       </c>
       <c r="C31" t="s">
-        <v>32</v>
+        <v>47</v>
       </c>
       <c r="D31" t="s">
         <v>46</v>
@@ -939,13 +951,13 @@
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A32">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C32" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D32" t="s">
-        <v>37</v>
+        <v>46</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.3">
@@ -953,7 +965,7 @@
         <v>8</v>
       </c>
       <c r="C33" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D33" t="s">
         <v>37</v>
@@ -964,7 +976,7 @@
         <v>8</v>
       </c>
       <c r="C34" t="s">
-        <v>19</v>
+        <v>34</v>
       </c>
       <c r="D34" t="s">
         <v>37</v>
@@ -975,7 +987,7 @@
         <v>8</v>
       </c>
       <c r="C35" t="s">
-        <v>35</v>
+        <v>19</v>
       </c>
       <c r="D35" t="s">
         <v>37</v>
@@ -986,10 +998,43 @@
         <v>8</v>
       </c>
       <c r="C36" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D36" t="s">
         <v>37</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A37">
+        <v>8</v>
+      </c>
+      <c r="C37" t="s">
+        <v>36</v>
+      </c>
+      <c r="D37" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A38">
+        <v>9</v>
+      </c>
+      <c r="C38" t="s">
+        <v>50</v>
+      </c>
+      <c r="D38" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A39">
+        <v>9</v>
+      </c>
+      <c r="C39" t="s">
+        <v>51</v>
+      </c>
+      <c r="D39" t="s">
+        <v>52</v>
       </c>
     </row>
   </sheetData>

</xml_diff>